<commit_message>
add contoh product price in example
</commit_message>
<xml_diff>
--- a/Data Product.xlsx
+++ b/Data Product.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dartmedia\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\laravel\apriori\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{425C7EBE-4D9B-4E37-BE34-33662472FD49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EA852B-AC43-4D4C-8267-CA3CACCA98A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{DE856B90-F240-4262-AF17-69A192DBE6E8}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{DE856B90-F240-4262-AF17-69A192DBE6E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Martabak Sultan Coklat Kacang</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Kode Product</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -546,269 +549,347 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B3" activeCellId="1" sqref="C11:C26 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3">
+        <v>100000</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4">
+        <v>100000</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5">
+        <v>100000</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6">
+        <v>100000</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
+      <c r="C7">
+        <v>100000</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
+      <c r="C8">
+        <v>100000</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="C9">
+        <v>100000</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10">
+        <v>100000</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
+      <c r="C11">
+        <v>100000</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
+      <c r="C12">
+        <v>100000</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
+      <c r="C13">
+        <v>100000</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
+      <c r="C14">
+        <v>100000</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
+      <c r="C15">
+        <v>100000</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
+      <c r="C16">
+        <v>100000</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
+      <c r="C17">
+        <v>100000</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
+      <c r="C18">
+        <v>100000</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
       </c>
+      <c r="C19">
+        <v>100000</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
       </c>
+      <c r="C20">
+        <v>100000</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>38</v>
       </c>
       <c r="B21" t="s">
         <v>39</v>
       </c>
+      <c r="C21">
+        <v>100000</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>40</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
       </c>
+      <c r="C22">
+        <v>100000</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>42</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
+      <c r="C23">
+        <v>100000</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>44</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
       </c>
+      <c r="C24">
+        <v>100000</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>47</v>
       </c>
+      <c r="C25">
+        <v>100000</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>48</v>
       </c>
       <c r="B26" t="s">
         <v>49</v>
+      </c>
+      <c r="C26">
+        <v>100000</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>

</xml_diff>